<commit_message>
Figured out issue. Unksporo was at 2 Sites (Mesquite and Creosote)  but marked for only being at one (Mesquite). Added row to edited-species4.csv, which solved issue. Wrote new clean subplot data csv
</commit_message>
<xml_diff>
--- a/data/raw/master-species_native.xlsx
+++ b/data/raw/master-species_native.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1449" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88FD981E-C713-4D26-A9FD-2B7EA8AA980B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
+    <workbookView minimized="1" xWindow="1860" yWindow="1872" windowWidth="17280" windowHeight="8880" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2618,8 +2618,8 @@
   <dimension ref="A1:D447"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <pane ySplit="1" topLeftCell="A413" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B426" sqref="B426"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Went back and made Genus spp. location-dependent; updated species lists but not subplot data yet
</commit_message>
<xml_diff>
--- a/data/raw/master-species_native.xlsx
+++ b/data/raw/master-species_native.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1449" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88FD981E-C713-4D26-A9FD-2B7EA8AA980B}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1860" yWindow="1872" windowWidth="17280" windowHeight="8880" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
+    <workbookView minimized="1" xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2618,8 +2618,8 @@
   <dimension ref="A1:D447"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A413" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B426" sqref="B426"/>
+      <pane ySplit="1" topLeftCell="A322" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B335" sqref="B335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Begin to continue 2x2 plot data wrangling
</commit_message>
<xml_diff>
--- a/data/raw/master-species_native.xlsx
+++ b/data/raw/master-species_native.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/04_RAMPS RestoreNet/RestoreNet/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1449" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{88FD981E-C713-4D26-A9FD-2B7EA8AA980B}"/>
+  <xr:revisionPtr revIDLastSave="1485" documentId="8_{FF5EA2F2-2FF6-42D4-ADD7-A9144DE3C437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB0599D4-0773-4A2E-B893-269E1F3E6490}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8880" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6ED14566-95D0-4DF3-9156-CD80DAE02F6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2262,7 +2262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2271,6 +2271,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2618,8 +2621,8 @@
   <dimension ref="A1:D447"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A322" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B335" sqref="B335"/>
+      <pane ySplit="1" topLeftCell="A440" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A407" activeCellId="1" sqref="A399:C399 A407:C407"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2778,7 +2781,7 @@
       <c r="B11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D11" t="s">
@@ -2848,7 +2851,7 @@
       <c r="B16" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D16" t="s">
@@ -2946,7 +2949,7 @@
       <c r="B23" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D23" t="s">
@@ -2960,7 +2963,7 @@
       <c r="B24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D24" t="s">
@@ -2974,7 +2977,7 @@
       <c r="B25" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D25" t="s">
@@ -3044,7 +3047,7 @@
       <c r="B30" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D30" t="s">
@@ -3212,7 +3215,7 @@
       <c r="B42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D42" t="s">
@@ -3310,7 +3313,7 @@
       <c r="B49" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D49" t="s">
@@ -3366,7 +3369,7 @@
       <c r="B53" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D53" t="s">
@@ -3450,7 +3453,7 @@
       <c r="B59" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D59" t="s">
@@ -3646,7 +3649,7 @@
       <c r="B73" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D73" t="s">
@@ -3828,7 +3831,7 @@
       <c r="B86" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D86" t="s">
@@ -3842,7 +3845,7 @@
       <c r="B87" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D87" t="s">
@@ -3884,7 +3887,7 @@
       <c r="B90" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D90" t="s">
@@ -3898,7 +3901,7 @@
       <c r="B91" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D91" t="s">
@@ -3996,7 +3999,7 @@
       <c r="B98" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C98" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D98" t="s">
@@ -4091,10 +4094,10 @@
       <c r="A105" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B105" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D105" t="s">
@@ -4105,10 +4108,10 @@
       <c r="A106" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B106" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C106" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D106" t="s">
@@ -4175,10 +4178,10 @@
       <c r="A111" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D111" t="s">
@@ -4259,10 +4262,10 @@
       <c r="A117" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="B117" t="s">
+      <c r="B117" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D117" t="s">
@@ -4329,10 +4332,10 @@
       <c r="A122" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B122" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C122" t="s">
+      <c r="C122" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D122" t="s">
@@ -4427,10 +4430,10 @@
       <c r="A129" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B129" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C129" t="s">
+      <c r="C129" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D129" t="s">
@@ -4441,10 +4444,10 @@
       <c r="A130" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B130" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C130" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D130" t="s">
@@ -4497,10 +4500,10 @@
       <c r="A134" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D134" t="s">
@@ -4539,10 +4542,10 @@
       <c r="A137" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B137" t="s">
+      <c r="B137" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D137" t="s">
@@ -4623,10 +4626,10 @@
       <c r="A143" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C143" t="s">
+      <c r="C143" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D143" t="s">
@@ -4651,10 +4654,10 @@
       <c r="A145" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C145" t="s">
+      <c r="C145" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D145" t="s">
@@ -4819,10 +4822,10 @@
       <c r="A157" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C157" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D157" t="s">
@@ -4833,10 +4836,10 @@
       <c r="A158" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C158" t="s">
+      <c r="C158" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D158" t="s">
@@ -4847,10 +4850,10 @@
       <c r="A159" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C159" t="s">
+      <c r="C159" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D159" t="s">
@@ -5166,13 +5169,13 @@
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A182" s="3" t="s">
+      <c r="A182" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B182" t="s">
+      <c r="B182" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C182" t="s">
+      <c r="C182" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D182" t="s">
@@ -5208,13 +5211,13 @@
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A185" s="3" t="s">
+      <c r="A185" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B185" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C185" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D185" t="s">
@@ -5390,13 +5393,13 @@
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A198" s="3" t="s">
+      <c r="A198" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="B198" t="s">
+      <c r="B198" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C198" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D198" t="s">
@@ -5404,13 +5407,13 @@
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A199" s="3" t="s">
+      <c r="A199" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B199" t="s">
+      <c r="B199" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C199" t="s">
+      <c r="C199" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D199" t="s">
@@ -5474,13 +5477,13 @@
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A204" s="3" t="s">
+      <c r="A204" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="B204" t="s">
+      <c r="B204" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="C204" t="s">
+      <c r="C204" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D204" t="s">
@@ -5572,13 +5575,13 @@
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A211" s="3" t="s">
+      <c r="A211" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="B211" t="s">
+      <c r="B211" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C211" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D211" t="s">
@@ -5740,13 +5743,13 @@
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A223" s="3" t="s">
+      <c r="A223" s="6" t="s">
         <v>382</v>
       </c>
-      <c r="B223" t="s">
+      <c r="B223" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="C223" t="s">
+      <c r="C223" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D223" t="s">
@@ -5754,13 +5757,13 @@
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A224" s="3" t="s">
+      <c r="A224" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="B224" t="s">
+      <c r="B224" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="C224" t="s">
+      <c r="C224" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D224" t="s">
@@ -5782,13 +5785,13 @@
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A226" s="3" t="s">
+      <c r="A226" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="B226" t="s">
+      <c r="B226" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="C226" t="s">
+      <c r="C226" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D226" t="s">
@@ -6006,13 +6009,13 @@
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A242" s="3" t="s">
+      <c r="A242" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="B242" t="s">
+      <c r="B242" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="C242" t="s">
+      <c r="C242" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D242" t="s">
@@ -6020,13 +6023,13 @@
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A243" s="3" t="s">
+      <c r="A243" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="B243" t="s">
+      <c r="B243" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C243" t="s">
+      <c r="C243" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D243" t="s">
@@ -6062,13 +6065,13 @@
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A246" s="3" t="s">
+      <c r="A246" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B246" t="s">
+      <c r="B246" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C246" t="s">
+      <c r="C246" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D246" t="s">
@@ -6076,13 +6079,13 @@
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A247" s="3" t="s">
+      <c r="A247" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="B247" t="s">
+      <c r="B247" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="C247" t="s">
+      <c r="C247" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D247" t="s">
@@ -6132,13 +6135,13 @@
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A251" s="3" t="s">
+      <c r="A251" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="B251" t="s">
+      <c r="B251" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C251" t="s">
+      <c r="C251" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D251" t="s">
@@ -6849,10 +6852,10 @@
       <c r="A302" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B302" t="s">
+      <c r="B302" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C302" t="s">
+      <c r="C302" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D302" t="s">
@@ -6863,10 +6866,10 @@
       <c r="A303" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="B303" t="s">
+      <c r="B303" s="1" t="s">
         <v>490</v>
       </c>
-      <c r="C303" t="s">
+      <c r="C303" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D303" t="s">
@@ -6877,10 +6880,10 @@
       <c r="A304" s="1" t="s">
         <v>491</v>
       </c>
-      <c r="B304" t="s">
+      <c r="B304" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="C304" t="s">
+      <c r="C304" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D304" t="s">
@@ -6902,13 +6905,13 @@
       </c>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A306" t="s">
+      <c r="A306" s="1" t="s">
         <v>495</v>
       </c>
-      <c r="B306" t="s">
+      <c r="B306" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="C306" t="s">
+      <c r="C306" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D306" t="s">
@@ -7143,10 +7146,10 @@
       <c r="A323" s="1" t="s">
         <v>512</v>
       </c>
-      <c r="B323" t="s">
+      <c r="B323" s="1" t="s">
         <v>513</v>
       </c>
-      <c r="C323" t="s">
+      <c r="C323" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D323" t="s">
@@ -7311,10 +7314,10 @@
       <c r="A335" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B335" t="s">
+      <c r="B335" s="1" t="s">
         <v>530</v>
       </c>
-      <c r="C335" t="s">
+      <c r="C335" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D335" t="s">
@@ -7353,10 +7356,10 @@
       <c r="A338" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="B338" t="s">
+      <c r="B338" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="C338" t="s">
+      <c r="C338" s="1" t="s">
         <v>699</v>
       </c>
       <c r="D338" t="s">

</xml_diff>